<commit_message>
More 2022 updates, waiting on GIS, API keys
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D420639A-9232-4C52-A94E-E3E2508E84D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898999EE-AAD6-404B-83AB-9F4FB1B85652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>ccao-condominium-pin_condo_char.R</t>
   </si>
   <si>
-    <t>ccao-condominium.R</t>
-  </si>
-  <si>
     <t>housing-ihs_index.R</t>
   </si>
   <si>
@@ -151,6 +148,33 @@
   </si>
   <si>
     <t>Needs to be run again early 2023</t>
+  </si>
+  <si>
+    <t>waiting to hear from Ray on subdivisions</t>
+  </si>
+  <si>
+    <t>waiting to hear from Josh on 2022 parcels</t>
+  </si>
+  <si>
+    <t>nothing to update, 12/14/22</t>
+  </si>
+  <si>
+    <t>waiting to hear from Josh on 21/22 school tax districts</t>
+  </si>
+  <si>
+    <t>waiting to hear from Josh on 21/22 tax districts</t>
+  </si>
+  <si>
+    <t>PACE feed no longer maintained</t>
+  </si>
+  <si>
+    <t>ccao-condominium_parking.R</t>
+  </si>
+  <si>
+    <t>waitin on valuations</t>
+  </si>
+  <si>
+    <t>waiting on great schools api</t>
   </si>
 </sst>
 </file>
@@ -518,7 +542,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,229 +556,262 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>44902</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
         <v>44902</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>44902</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>44907</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>44902</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>44903</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44909</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1">
         <v>44902</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1"/>
     </row>

</xml_diff>

<commit_message>
Bump deps, change script names, update inventory
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898999EE-AAD6-404B-83AB-9F4FB1B85652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E053CA-A73F-4D8A-BC2E-B504EEF9793E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>ccao-condominium-pin_condo_char.R</t>
   </si>
@@ -147,9 +147,6 @@
     <t>deprectaed, 12/8/22</t>
   </si>
   <si>
-    <t>Needs to be run again early 2023</t>
-  </si>
-  <si>
     <t>waiting to hear from Ray on subdivisions</t>
   </si>
   <si>
@@ -171,10 +168,79 @@
     <t>ccao-condominium_parking.R</t>
   </si>
   <si>
-    <t>waitin on valuations</t>
-  </si>
-  <si>
     <t>waiting on great schools api</t>
+  </si>
+  <si>
+    <t>needs to be run again early 2023</t>
+  </si>
+  <si>
+    <t>ccao-dictionary.R</t>
+  </si>
+  <si>
+    <t>ccao-land-land_nbhd_rate.R</t>
+  </si>
+  <si>
+    <t>ccao-land-land_site_rate.R</t>
+  </si>
+  <si>
+    <t>ccao-other-hie.R</t>
+  </si>
+  <si>
+    <t>census-acs.R</t>
+  </si>
+  <si>
+    <t>census-decennial.R</t>
+  </si>
+  <si>
+    <t>census-dictionary.R</t>
+  </si>
+  <si>
+    <t>environment-airport_noise.R</t>
+  </si>
+  <si>
+    <t>environment-flood_first_street.R</t>
+  </si>
+  <si>
+    <t>export-geojson.R</t>
+  </si>
+  <si>
+    <t>spatial-ccao-county.R</t>
+  </si>
+  <si>
+    <t>spatial-ccao-neighborhood.R</t>
+  </si>
+  <si>
+    <t>spatial-ccao-township.R</t>
+  </si>
+  <si>
+    <t>spatial-environment-golf_course.R</t>
+  </si>
+  <si>
+    <t>spatial-environment-major_road.R</t>
+  </si>
+  <si>
+    <t>spatial-environment-midway_noise.R</t>
+  </si>
+  <si>
+    <t>tax-ptaxsim.R</t>
+  </si>
+  <si>
+    <t>no need to update, 12/15/22</t>
+  </si>
+  <si>
+    <t>waiting on valuations, 12/15/22</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>no new data available</t>
+  </si>
+  <si>
+    <t>waiting on decision vis-à-vis smartfile</t>
+  </si>
+  <si>
+    <t>needs to be run again early 2023(?)</t>
   </si>
 </sst>
 </file>
@@ -195,12 +261,18 @@
       <name val="JetBrains Mono"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -224,6 +296,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,9 +613,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E138CF-54D8-4F6E-9B04-C9597DC88E9C}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +623,7 @@
     <col min="1" max="1" width="43.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -571,17 +644,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>44</v>
+      <c r="D2" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -634,7 +707,7 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -647,7 +720,9 @@
       <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -657,12 +732,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
-        <v>45</v>
+      <c r="D10" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -689,11 +764,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -721,11 +796,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -737,20 +812,20 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -758,7 +833,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -773,20 +848,20 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -800,7 +875,7 @@
         <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,14 +898,289 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5475F86-C267-4D66-A7A8-8A1BD6C317DA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44910</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44910</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44910</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last round of updates for now, waiting on several parties
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E053CA-A73F-4D8A-BC2E-B504EEF9793E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F141790-5EE2-485C-86F5-FC9A8AC1DCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
   <si>
     <t>ccao-condominium-pin_condo_char.R</t>
   </si>
@@ -138,12 +138,6 @@
     <t>no need to update, 12/8/22</t>
   </si>
   <si>
-    <t>census shapefiles for 2022 not yet available 12/8/22</t>
-  </si>
-  <si>
-    <t>tigris not yet updated with 2022 data</t>
-  </si>
-  <si>
     <t>deprectaed, 12/8/22</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>ccao-condominium_parking.R</t>
   </si>
   <si>
-    <t>waiting on great schools api</t>
-  </si>
-  <si>
     <t>needs to be run again early 2023</t>
   </si>
   <si>
@@ -241,13 +232,40 @@
   </si>
   <si>
     <t>needs to be run again early 2023(?)</t>
+  </si>
+  <si>
+    <t>waiting to hear from Josh on railroads (everything else is done)</t>
+  </si>
+  <si>
+    <t>nothing to update 12/19/22</t>
+  </si>
+  <si>
+    <t>2020 acs1 data not included</t>
+  </si>
+  <si>
+    <t>no need to update, 12/19/22</t>
+  </si>
+  <si>
+    <t>waiting on josh, 12/19/22</t>
+  </si>
+  <si>
+    <t>nothing to update, 12/19/22</t>
+  </si>
+  <si>
+    <t>waiting on valuations, 12/20/22</t>
+  </si>
+  <si>
+    <t>waiting on…?</t>
+  </si>
+  <si>
+    <t>nothing to update, 12/20/22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +277,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="JetBrains Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -287,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -297,6 +320,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +640,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,12 +674,12 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -707,7 +732,7 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -721,7 +746,7 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,15 +754,15 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>43</v>
+      <c r="D10" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -764,12 +789,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>33</v>
+      <c r="B14" s="1">
+        <v>44911</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -788,7 +816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -796,15 +824,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -812,31 +840,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -848,23 +876,23 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -875,10 +903,10 @@
         <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -900,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5475F86-C267-4D66-A7A8-8A1BD6C317DA}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,85 +958,109 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>63</v>
+      <c r="D2" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
+      <c r="D7" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44914</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44914</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>54</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1022,18 +1074,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
-        <v>66</v>
+      <c r="D15" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
+      <c r="B16" s="1">
+        <v>44907</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1046,12 +1107,15 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>6</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,7 +1129,7 @@
         <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,100 +1150,176 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="B25" s="6">
+        <v>44914</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>59</v>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="6">
+        <v>44915</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="D31" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D32" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B35" s="1">
+        <v>44903</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="D36" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D37" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
+        <v>44915</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
+        <v>44914</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor update to inventory
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F141790-5EE2-485C-86F5-FC9A8AC1DCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D15A198-5DD9-444C-88EA-C0D00DC889EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
@@ -310,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -320,8 +320,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,7 +638,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,11 +755,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>66</v>
       </c>
     </row>
@@ -929,7 +927,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,14 +1170,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="1">
         <v>44914</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1191,22 +1189,22 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="1">
         <v>44915</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1289,10 +1287,10 @@
       <c r="A38" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="1">
         <v>44915</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" t="s">
         <v>28</v>
       </c>
       <c r="D38" t="s">
@@ -1303,10 +1301,10 @@
       <c r="A39" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="1">
         <v>44914</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Resolve "Rewrite raw ingest scripts for county gdb files"
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D15A198-5DD9-444C-88EA-C0D00DC889EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B095FBB5-6E0C-4ADF-A0D5-282824EB1714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -310,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -320,6 +320,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +640,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,72 +824,87 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B18" s="6">
+        <v>44924</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="B20" s="6">
+        <v>44924</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B21" s="6">
+        <v>44924</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="6">
         <v>44903</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="C23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="B24" s="6">
+        <v>44924</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>38</v>
+      <c r="B25" s="6">
+        <v>44924</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -927,7 +944,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Done with warehouse updates for now
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B095FBB5-6E0C-4ADF-A0D5-282824EB1714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC679F3-5F6E-4F21-A1CF-730ED11D2AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
   <si>
     <t>ccao-condominium-pin_condo_char.R</t>
   </si>
@@ -234,9 +234,6 @@
     <t>needs to be run again early 2023(?)</t>
   </si>
   <si>
-    <t>waiting to hear from Josh on railroads (everything else is done)</t>
-  </si>
-  <si>
     <t>nothing to update 12/19/22</t>
   </si>
   <si>
@@ -259,6 +256,9 @@
   </si>
   <si>
     <t>nothing to update, 12/20/22</t>
+  </si>
+  <si>
+    <t>1/11/20203</t>
   </si>
 </sst>
 </file>
@@ -320,8 +320,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,7 +764,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -824,86 +826,86 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="1">
         <v>44924</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="C18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="1">
         <v>44924</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="1">
         <v>44924</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="1">
         <v>44903</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="C23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="1">
         <v>44924</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="1">
         <v>44924</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -943,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5475F86-C267-4D66-A7A8-8A1BD6C317DA}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1020,7 @@
         <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1032,7 +1034,7 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1040,7 +1042,7 @@
         <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,7 +1077,7 @@
         <v>51</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,7 +1132,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,7 +1213,7 @@
         <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,27 +1243,42 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="B31" s="1">
+        <v>44925</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="B32" s="1">
+        <v>44925</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="B33" s="1">
+        <v>44931</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1270,7 +1287,7 @@
         <v>19</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1278,7 +1295,7 @@
         <v>20</v>
       </c>
       <c r="B35" s="1">
-        <v>44903</v>
+        <v>44566</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -1288,6 +1305,12 @@
       <c r="A36" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="B36" s="5">
+        <v>44936</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="D36" s="4" t="s">
         <v>37</v>
       </c>
@@ -1296,6 +1319,12 @@
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B37" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="D37" s="4" t="s">
         <v>38</v>
       </c>
@@ -1330,7 +1359,7 @@
         <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor updates to address CTAS issues
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC679F3-5F6E-4F21-A1CF-730ED11D2AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F5BFC3-5486-4193-949D-A2CAD6F2AB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Warehouse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="69">
   <si>
     <t>ccao-condominium-pin_condo_char.R</t>
   </si>
@@ -141,21 +142,9 @@
     <t>deprectaed, 12/8/22</t>
   </si>
   <si>
-    <t>waiting to hear from Ray on subdivisions</t>
-  </si>
-  <si>
-    <t>waiting to hear from Josh on 2022 parcels</t>
-  </si>
-  <si>
     <t>nothing to update, 12/14/22</t>
   </si>
   <si>
-    <t>waiting to hear from Josh on 21/22 school tax districts</t>
-  </si>
-  <si>
-    <t>waiting to hear from Josh on 21/22 tax districts</t>
-  </si>
-  <si>
     <t>PACE feed no longer maintained</t>
   </si>
   <si>
@@ -241,9 +230,6 @@
   </si>
   <si>
     <t>no need to update, 12/19/22</t>
-  </si>
-  <si>
-    <t>waiting on josh, 12/19/22</t>
   </si>
   <si>
     <t>nothing to update, 12/19/22</t>
@@ -310,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -320,10 +306,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,7 +618,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -642,7 +630,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,12 +664,12 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -723,32 +711,32 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="6">
         <v>44907</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="6">
         <v>44902</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>64</v>
+      <c r="C8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -764,7 +752,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -872,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,7 +908,7 @@
         <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -945,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5475F86-C267-4D66-A7A8-8A1BD6C317DA}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,52 +968,52 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1">
         <v>44914</v>
@@ -1034,20 +1022,20 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1">
         <v>44914</v>
@@ -1058,26 +1046,29 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="8">
+        <v>44573</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1096,7 +1087,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1110,7 +1101,7 @@
         <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1124,7 +1115,7 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1132,7 +1123,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,7 +1137,7 @@
         <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,7 +1158,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
@@ -1175,7 +1166,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
@@ -1183,7 +1174,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>31</v>
@@ -1210,15 +1201,15 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1">
         <v>44915</v>
@@ -1229,7 +1220,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1264,9 +1255,6 @@
       <c r="C32" t="s">
         <v>28</v>
       </c>
-      <c r="D32" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1278,16 +1266,13 @@
       <c r="C33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D33" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,32 +1286,26 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="1">
         <v>44936</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>38</v>
+      <c r="B37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1340,7 +1319,7 @@
         <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,10 +1335,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update inventory updated with new sales script runs for early 2023
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F5BFC3-5486-4193-949D-A2CAD6F2AB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE2329B-1751-48F7-B391-BC15C6FF1C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Warehouse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="69">
   <si>
     <t>ccao-condominium-pin_condo_char.R</t>
   </si>
@@ -618,7 +617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -934,7 +933,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,12 +962,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>56</v>
+      <c r="B2" s="8">
+        <v>44979</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1060,14 +1059,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="1">
         <v>44573</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1095,13 +1094,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1">
-        <v>44907</v>
+        <v>44984</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1109,13 +1105,10 @@
         <v>5</v>
       </c>
       <c r="B17" s="1">
-        <v>44910</v>
+        <v>44984</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First sweep of 23 updates
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE2329B-1751-48F7-B391-BC15C6FF1C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4B027D-835F-4661-A0A2-23140B8FF167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
   <si>
     <t>ccao-condominium-pin_condo_char.R</t>
   </si>
@@ -138,9 +138,6 @@
     <t>no need to update, 12/8/22</t>
   </si>
   <si>
-    <t>deprectaed, 12/8/22</t>
-  </si>
-  <si>
     <t>nothing to update, 12/14/22</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>ccao-condominium_parking.R</t>
   </si>
   <si>
-    <t>needs to be run again early 2023</t>
-  </si>
-  <si>
     <t>ccao-dictionary.R</t>
   </si>
   <si>
@@ -219,12 +213,6 @@
     <t>waiting on decision vis-à-vis smartfile</t>
   </si>
   <si>
-    <t>needs to be run again early 2023(?)</t>
-  </si>
-  <si>
-    <t>nothing to update 12/19/22</t>
-  </si>
-  <si>
     <t>2020 acs1 data not included</t>
   </si>
   <si>
@@ -244,6 +232,24 @@
   </si>
   <si>
     <t>1/11/20203</t>
+  </si>
+  <si>
+    <t>spatial-environment-golf_course.py</t>
+  </si>
+  <si>
+    <t>waiting on field, 10/04/23</t>
+  </si>
+  <si>
+    <t>no need to update, 10/04/23</t>
+  </si>
+  <si>
+    <t>2017 data no longer available, should we delete?</t>
+  </si>
+  <si>
+    <t>no need to update, 10/05/23</t>
+  </si>
+  <si>
+    <t>nothing to update, 10/05/23</t>
   </si>
 </sst>
 </file>
@@ -295,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -309,8 +315,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,11 +629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E138CF-54D8-4F6E-9B04-C9597DC88E9C}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD8"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,15 +667,18 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45183</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -679,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>44902</v>
+        <v>45203</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -690,111 +697,92 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>44902</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
-        <v>44902</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
-        <v>44907</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
-        <v>44902</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44911</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -817,12 +805,8 @@
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1">
-        <v>44924</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -836,91 +820,59 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="1">
-        <v>44924</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="1">
-        <v>44924</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="1">
-        <v>44903</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="1">
-        <v>44924</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="1">
-        <v>44924</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="1">
-        <v>44909</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
-      </c>
+      <c r="B26" s="1"/>
       <c r="D26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="1">
-        <v>44902</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2032733072</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -932,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5475F86-C267-4D66-A7A8-8A1BD6C317DA}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,57 +914,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="1">
         <v>44979</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1">
         <v>44914</v>
@@ -1021,20 +973,20 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1">
         <v>44914</v>
@@ -1045,23 +997,23 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1">
         <v>44573</v>
@@ -1086,7 +1038,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1116,7 +1068,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1130,7 +1082,7 @@
         <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,7 +1103,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
@@ -1159,7 +1111,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
@@ -1167,7 +1119,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
         <v>31</v>
@@ -1194,15 +1146,15 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1">
         <v>44915</v>
@@ -1213,7 +1165,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1265,7 +1217,7 @@
         <v>19</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
         <v>28</v>
@@ -1312,7 +1264,7 @@
         <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,10 +1280,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Just waiting on sales and condo chars
</commit_message>
<xml_diff>
--- a/aws-s3/update_inventory.xlsx
+++ b/aws-s3/update_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\data-architecture\aws-s3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D776D193-0502-4D87-AA6E-EDD74A14474C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AF98D0-596F-4856-BF79-8B7ABF986F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35985" yWindow="1020" windowWidth="21600" windowHeight="13890" activeTab="2" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
+    <workbookView xWindow="31950" yWindow="1920" windowWidth="23565" windowHeight="13560" xr2:uid="{1C446241-3B2D-4EFC-B595-695EA445075D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -669,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -687,6 +687,8 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,9 +1005,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E138CF-54D8-4F6E-9B04-C9597DC88E9C}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1085,13 +1087,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:5" s="11" customFormat="1">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="12">
+        <v>45301</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1326,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5475F86-C267-4D66-A7A8-8A1BD6C317DA}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1396,11 +1402,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:5" s="11" customFormat="1">
+      <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="B6" s="12">
+        <v>45300</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1502,18 +1511,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="4" customFormat="1">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:4" s="11" customFormat="1">
+      <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="5">
-        <v>44984</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="12">
+        <v>45301</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1">
@@ -1771,7 +1777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA852B2-127D-4B3A-8504-0AB427458A62}">
   <dimension ref="A1:E225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>

</xml_diff>